<commit_message>
menambahkan gambar dan memperbaiki bug
</commit_message>
<xml_diff>
--- a/Product Backlog+User Story.xlsx
+++ b/Product Backlog+User Story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agile uas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4116A3-8668-4992-B348-3D08046ABE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF82F8FD-416F-4C1C-9088-8C7697EDA2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -998,15 +998,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1033,9 +1030,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1076,77 +1070,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1157,21 +1166,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1180,6 +1174,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1741,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B8536-4987-4D23-A1DF-107BD88A4060}">
   <dimension ref="B1:I131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80:H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1758,24 +1755,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>211110476</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>69</v>
       </c>
       <c r="F3" t="s">
@@ -1783,558 +1780,558 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>211110404</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>211110443</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="41" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="46">
+      <c r="B9" s="56">
         <v>5</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="33">
         <v>5</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="35" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="48"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="53" t="s">
+      <c r="B10" s="46"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="33">
         <v>5</v>
       </c>
-      <c r="I10" s="42"/>
+      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="45">
         <v>6</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="44" t="s">
+      <c r="C11" s="52"/>
+      <c r="D11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>5</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="48"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="53" t="s">
+      <c r="B12" s="46"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>5</v>
       </c>
-      <c r="I12" s="41"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="45">
         <v>8</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="66" t="s">
+      <c r="G13" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>8</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="48"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="53" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>8</v>
       </c>
-      <c r="I14" s="41"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="45">
         <v>4</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="44" t="s">
+      <c r="C15" s="52"/>
+      <c r="D15" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="66" t="s">
+      <c r="G15" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>8</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="48"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="53" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>8</v>
       </c>
-      <c r="I16" s="41"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="45">
         <v>11</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>5</v>
       </c>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="48"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="53" t="s">
+      <c r="B18" s="46"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="E18" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>5</v>
       </c>
-      <c r="I18" s="41"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="45">
         <v>2</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="44" t="s">
+      <c r="C19" s="52"/>
+      <c r="D19" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>5</v>
       </c>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="48"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="53" t="s">
+      <c r="B20" s="46"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>5</v>
       </c>
-      <c r="I20" s="41"/>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="45">
         <v>3</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="44" t="s">
+      <c r="C21" s="52"/>
+      <c r="D21" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="66" t="s">
+      <c r="G21" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>8</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="34" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="48"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="53" t="s">
+      <c r="B22" s="46"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="66" t="s">
+      <c r="G22" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>8</v>
       </c>
-      <c r="I22" s="41"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="45">
         <v>10</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="44" t="s">
+      <c r="C23" s="52"/>
+      <c r="D23" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="66" t="s">
+      <c r="G23" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>5</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="34" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="24" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="48"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="53" t="s">
+      <c r="B24" s="46"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="G24" s="66" t="s">
+      <c r="G24" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <v>5</v>
       </c>
-      <c r="I24" s="41"/>
+      <c r="I24" s="34"/>
     </row>
     <row r="25" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="45">
         <v>1</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="66" t="s">
+      <c r="G25" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="3">
         <v>13</v>
       </c>
-      <c r="I25" s="41" t="s">
+      <c r="I25" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="48"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="53" t="s">
+      <c r="B26" s="46"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="49" t="s">
+      <c r="E26" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="66" t="s">
+      <c r="G26" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <v>13</v>
       </c>
-      <c r="I26" s="41"/>
+      <c r="I26" s="34"/>
     </row>
     <row r="27" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="45">
         <v>9</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="66" t="s">
+      <c r="G27" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <v>3</v>
       </c>
-      <c r="I27" s="41" t="s">
+      <c r="I27" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="48"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="53" t="s">
+      <c r="B28" s="46"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="49" t="s">
+      <c r="F28" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="G28" s="66" t="s">
+      <c r="G28" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <v>3</v>
       </c>
-      <c r="I28" s="41"/>
+      <c r="I28" s="34"/>
     </row>
     <row r="29" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="45">
         <v>7</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="66" t="s">
+      <c r="G29" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <v>21</v>
       </c>
-      <c r="I29" s="41" t="s">
+      <c r="I29" s="34" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="48"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="53" t="s">
+      <c r="B30" s="46"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="49" t="s">
+      <c r="E30" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="G30" s="66" t="s">
+      <c r="G30" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>21</v>
       </c>
-      <c r="I30" s="41"/>
+      <c r="I30" s="34"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D31" s="1"/>
@@ -2347,1022 +2344,1040 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="24"/>
-      <c r="C33" s="25" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="27"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="25"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="29"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="27"/>
+      <c r="C34" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="18"/>
-      <c r="H34" s="19"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
       </c>
-      <c r="H35" s="20"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="30">
+      <c r="B36" s="28">
         <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="20"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="30">
+      <c r="B37" s="28">
         <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="20"/>
+      <c r="H37" s="18"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="20"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="31">
+      <c r="B39" s="29">
         <v>1</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
     </row>
     <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="41" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="16"/>
-      <c r="C41" s="18" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18" t="s">
+      <c r="D41" s="16"/>
+      <c r="E41" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F41" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="18"/>
-      <c r="H41" s="19"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="27"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="25"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="30">
+      <c r="B43" s="28">
         <v>1</v>
       </c>
       <c r="C43" t="s">
         <v>33</v>
       </c>
-      <c r="H43" s="20"/>
+      <c r="H43" s="18"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="30">
+      <c r="B44" s="28">
         <v>2</v>
       </c>
       <c r="C44" t="s">
         <v>34</v>
       </c>
-      <c r="H44" s="20"/>
+      <c r="H44" s="18"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="30">
+      <c r="B45" s="28">
         <v>3</v>
       </c>
       <c r="C45" t="s">
         <v>41</v>
       </c>
-      <c r="H45" s="20"/>
+      <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="H46" s="20"/>
+      <c r="H46" s="18"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="30">
+      <c r="B47" s="28">
         <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
       </c>
-      <c r="H47" s="20"/>
+      <c r="H47" s="18"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="30">
+      <c r="B48" s="28">
         <v>6</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="20"/>
+      <c r="H48" s="18"/>
     </row>
     <row r="49" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="31">
+      <c r="B49" s="29">
         <v>9</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="23"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="21"/>
     </row>
     <row r="50" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="16"/>
-      <c r="C51" s="18" t="s">
+      <c r="B51" s="14"/>
+      <c r="C51" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18" t="s">
+      <c r="D51" s="16"/>
+      <c r="E51" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="19"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="17"/>
     </row>
     <row r="52" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="27"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="25"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="30">
+      <c r="B53" s="28">
         <v>1</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="20"/>
+      <c r="H53" s="18"/>
     </row>
     <row r="54" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="30">
+      <c r="B54" s="28">
         <v>2</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H54" s="20"/>
+      <c r="H54" s="18"/>
     </row>
     <row r="55" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="30">
+      <c r="B55" s="28">
         <v>3</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H55" s="20"/>
+      <c r="H55" s="18"/>
     </row>
     <row r="56" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="30">
+      <c r="B56" s="28">
         <v>4</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H56" s="20"/>
+      <c r="H56" s="18"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C57" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="20"/>
+      <c r="H57" s="18"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B58" s="32">
+      <c r="B58" s="30">
         <v>8</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="20"/>
+      <c r="H58" s="18"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B59" s="32">
+      <c r="B59" s="30">
         <v>4</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H59" s="20"/>
+      <c r="H59" s="18"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B60" s="32">
+      <c r="B60" s="30">
         <v>11</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="20"/>
+      <c r="H60" s="18"/>
     </row>
     <row r="61" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="33">
+      <c r="B61" s="31">
         <v>2</v>
       </c>
-      <c r="C61" s="28" t="s">
+      <c r="C61" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="23"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="21"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B62" s="6"/>
+      <c r="B62" s="5"/>
       <c r="C62" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D64" s="57"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="58"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="50"/>
+      <c r="H64" s="51"/>
     </row>
     <row r="65" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C66" s="2">
+      <c r="C66" s="4">
         <v>1</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F66" s="13">
+      <c r="F66" s="68">
         <v>45043</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H66" s="13">
+      <c r="H66" s="68">
         <v>45043</v>
       </c>
     </row>
     <row r="67" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C67" s="2">
+      <c r="C67" s="4">
         <v>2</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F67" s="13">
+      <c r="F67" s="68">
         <v>45043</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H67" s="13">
+      <c r="H67" s="68">
         <v>45043</v>
       </c>
     </row>
     <row r="68" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C68" s="2">
+      <c r="C68" s="4">
         <v>3</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="13">
+      <c r="F68" s="68">
         <v>45043</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H68" s="13">
+      <c r="H68" s="68">
         <v>45043</v>
       </c>
     </row>
     <row r="69" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C69" s="2">
+      <c r="C69" s="4">
         <v>4</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F69" s="13">
+      <c r="F69" s="68">
         <v>45044</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H69" s="13">
+      <c r="H69" s="68">
         <v>45044</v>
       </c>
     </row>
     <row r="70" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C70" s="2">
+      <c r="C70" s="4">
         <v>5</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F70" s="13">
+      <c r="F70" s="68">
         <v>45044</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H70" s="13">
+      <c r="H70" s="68">
         <v>45044</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C71" s="2">
+      <c r="C71" s="4">
         <v>6</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F71" s="13">
+      <c r="F71" s="68">
         <v>45045</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H71" s="13">
+      <c r="H71" s="68">
         <v>45045</v>
       </c>
     </row>
     <row r="72" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C72" s="2">
+      <c r="C72" s="4">
         <v>7</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F72" s="13">
+      <c r="F72" s="68">
         <v>45045</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H72" s="13">
+      <c r="H72" s="68">
         <v>45045</v>
       </c>
     </row>
     <row r="73" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C73" s="2">
+      <c r="C73" s="4">
         <v>8</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F73" s="13">
+      <c r="F73" s="68">
         <v>45046</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H73" s="13">
+      <c r="H73" s="68">
         <v>45046</v>
       </c>
     </row>
     <row r="74" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C74" s="2">
+      <c r="C74" s="4">
         <v>9</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F74" s="13">
+      <c r="F74" s="68">
         <v>45046</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H74" s="13">
+      <c r="H74" s="68">
         <v>45046</v>
       </c>
     </row>
     <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C75" s="2">
+      <c r="C75" s="4">
         <v>10</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F75" s="13">
+      <c r="F75" s="68">
         <v>45047</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H75" s="13">
+      <c r="H75" s="68">
         <v>45047</v>
       </c>
     </row>
     <row r="76" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C76" s="2">
+      <c r="C76" s="4">
         <v>11</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F76" s="13">
+      <c r="F76" s="68">
         <v>45048</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H76" s="13">
+      <c r="H76" s="68">
         <v>45048</v>
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C77" s="2">
+      <c r="C77" s="4">
         <v>12</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F77" s="13">
+      <c r="F77" s="68">
         <v>45049</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G77" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H77" s="13">
+      <c r="H77" s="68">
         <v>45049</v>
       </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C79" s="38" t="s">
+      <c r="C79" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D79" s="38"/>
-      <c r="E79" s="38"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="59"/>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="D80" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E80" s="10" t="s">
+      <c r="E80" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C81" s="36" t="s">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C81" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-    </row>
-    <row r="82" spans="3:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="C82" s="8" t="s">
+      <c r="D81" s="58"/>
+      <c r="E81" s="58"/>
+    </row>
+    <row r="82" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C82" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D82" s="12" t="s">
+      <c r="D82" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C83" s="36" t="s">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C83" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-    </row>
-    <row r="84" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C84" s="8" t="s">
+      <c r="D83" s="58"/>
+      <c r="E83" s="58"/>
+    </row>
+    <row r="84" spans="3:6" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="C84" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="85" spans="3:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="C85" s="8" t="s">
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C85" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E85" s="8"/>
-    </row>
-    <row r="86" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C86" s="8" t="s">
+      <c r="E85" s="7"/>
+    </row>
+    <row r="86" spans="3:6" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="C86" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E86" s="8"/>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C87" s="36" t="s">
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C87" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
-    </row>
-    <row r="88" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C88" s="8" t="s">
+      <c r="D87" s="58"/>
+      <c r="E87" s="58"/>
+    </row>
+    <row r="88" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C88" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D88" s="9" t="s">
+      <c r="D88" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="3:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="C89" s="11"/>
-      <c r="D89" s="9" t="s">
+    <row r="89" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C89" s="10"/>
+      <c r="D89" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E89" s="11"/>
-    </row>
-    <row r="90" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C90" s="11"/>
-      <c r="D90" s="9" t="s">
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C90" s="10"/>
+      <c r="D90" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E90" s="11"/>
-    </row>
-    <row r="91" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C91" s="11"/>
-      <c r="D91" s="9" t="s">
+      <c r="E90" s="10"/>
+    </row>
+    <row r="91" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C91" s="10"/>
+      <c r="D91" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="11"/>
-    </row>
-    <row r="92" spans="3:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="C92" s="59" t="s">
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" spans="3:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="C92" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="D92" s="60"/>
-      <c r="E92" s="61"/>
-    </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C93" s="67" t="s">
+      <c r="D92" s="63"/>
+      <c r="E92" s="64"/>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="D93" s="68"/>
-      <c r="E93" s="69"/>
-    </row>
-    <row r="94" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C94" s="9" t="s">
+      <c r="D93" s="66"/>
+      <c r="E93" s="67"/>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C94" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D94" s="9" t="s">
+      <c r="D94" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="95" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C95" s="9" t="s">
+    <row r="95" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C95" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D95" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E95" s="11"/>
-    </row>
-    <row r="96" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C96" s="9" t="s">
+      <c r="E95" s="10"/>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C96" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D96" s="9" t="s">
+      <c r="D96" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E96" s="11"/>
-    </row>
-    <row r="97" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C97" s="9" t="s">
+      <c r="E96" s="10"/>
+    </row>
+    <row r="97" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C97" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D97" s="9"/>
-      <c r="E97" s="11"/>
-    </row>
-    <row r="98" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C98" s="9" t="s">
+      <c r="D97" s="8"/>
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C98" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D98" s="9"/>
-      <c r="E98" s="11"/>
-    </row>
-    <row r="99" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C99" s="9" t="s">
+      <c r="D98" s="8"/>
+      <c r="E98" s="10"/>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C99" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D99" s="9"/>
-      <c r="E99" s="11"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C100" s="67" t="s">
+      <c r="C100" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="D100" s="68"/>
-      <c r="E100" s="69"/>
+      <c r="D100" s="66"/>
+      <c r="E100" s="67"/>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C101" s="7"/>
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C103" s="39" t="s">
+      <c r="C103" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="D103" s="39"/>
-      <c r="E103" s="39"/>
-      <c r="F103" s="39"/>
-      <c r="G103" s="39"/>
+      <c r="D103" s="61"/>
+      <c r="E103" s="61"/>
+      <c r="F103" s="61"/>
+      <c r="G103" s="61"/>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C104" s="37" t="s">
+      <c r="C104" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D104" s="37"/>
-      <c r="E104" s="37" t="s">
+      <c r="D104" s="60"/>
+      <c r="E104" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="F104" s="37"/>
-      <c r="G104" s="37"/>
+      <c r="F104" s="60"/>
+      <c r="G104" s="60"/>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C105" s="14" t="s">
+      <c r="C105" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D105" s="14" t="s">
+      <c r="D105" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E105" s="14" t="s">
+      <c r="E105" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F105" s="14" t="s">
+      <c r="F105" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G105" s="14" t="s">
+      <c r="G105" s="12" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C106" s="35" t="s">
+      <c r="C106" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D106" s="35"/>
-      <c r="E106" s="35"/>
-      <c r="F106" s="35"/>
-      <c r="G106" s="35"/>
-    </row>
-    <row r="107" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C107" s="5" t="s">
+      <c r="D106" s="44"/>
+      <c r="E106" s="44"/>
+      <c r="F106" s="44"/>
+      <c r="G106" s="44"/>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C107" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E107" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F107" s="3" t="s">
+      <c r="F107" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="G107" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="108" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="5" t="s">
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C109" s="35" t="s">
+      <c r="C109" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D109" s="35"/>
-      <c r="E109" s="35"/>
-      <c r="F109" s="35"/>
-      <c r="G109" s="35"/>
-    </row>
-    <row r="110" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C110" s="5" t="s">
+      <c r="D109" s="44"/>
+      <c r="E109" s="44"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="44"/>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C110" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E110" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F110" s="3" t="s">
+      <c r="F110" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="G110" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="111" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C111" s="5" t="s">
+      <c r="C111" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
-      <c r="F111" s="5" t="s">
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G111" s="3"/>
+      <c r="G111" s="2"/>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C112" s="35" t="s">
+      <c r="C112" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D112" s="35"/>
-      <c r="E112" s="35"/>
-      <c r="F112" s="35"/>
-      <c r="G112" s="35"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
     </row>
     <row r="113" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C113" s="5" t="s">
+      <c r="C113" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3" t="s">
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G113" s="3"/>
+      <c r="G113" s="2"/>
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C116" s="35" t="s">
+      <c r="C116" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="D116" s="35"/>
-      <c r="E116" s="35"/>
-      <c r="F116" s="35"/>
-      <c r="G116" s="35"/>
+      <c r="D116" s="44"/>
+      <c r="E116" s="44"/>
+      <c r="F116" s="44"/>
+      <c r="G116" s="44"/>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E117" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F117" s="3" t="s">
+      <c r="F117" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G117" s="3" t="s">
+      <c r="G117" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="6"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
     </row>
     <row r="121" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C121" s="6" t="s">
+      <c r="C121" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="6"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="6"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="6"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
-      <c r="E125" s="6"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="6"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="6"/>
-      <c r="F127" s="6"/>
-      <c r="G127" s="6"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="6"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+      <c r="G128" s="5"/>
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C131" s="6"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="6"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="6"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="C116:G116"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
@@ -3373,29 +3388,12 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C109:G109"/>
     <mergeCell ref="C112:G112"/>
     <mergeCell ref="C106:G106"/>
     <mergeCell ref="C87:E87"/>
     <mergeCell ref="C104:D104"/>
     <mergeCell ref="E104:G104"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C100:E100"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:G30">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="medium">

</xml_diff>

<commit_message>
sprint 6 sudah selesai
</commit_message>
<xml_diff>
--- a/Product Backlog+User Story.xlsx
+++ b/Product Backlog+User Story.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agile uas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agile biasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475725BA-B0DD-4E8B-BFCF-D254DB2AA441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F020C32-1205-4F93-A792-B00D9DA77C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="195">
   <si>
     <t>ID</t>
   </si>
@@ -459,9 +459,6 @@
     <t>Cart Function</t>
   </si>
   <si>
-    <t>Meetig berjalan dengan lancar</t>
-  </si>
-  <si>
     <t>Meeting berhasil dilaksanakan</t>
   </si>
   <si>
@@ -513,9 +510,6 @@
     <t>Supaya user dapat mengorder pesanan yang sudah dibuat</t>
   </si>
   <si>
-    <t>on progress</t>
-  </si>
-  <si>
     <t>Dimulai setelah UTS</t>
   </si>
   <si>
@@ -580,6 +574,45 @@
   </si>
   <si>
     <t>tombol back belum berfungsi dengan baik</t>
+  </si>
+  <si>
+    <t>Fitur Notification Pages sudah diterapkan</t>
+  </si>
+  <si>
+    <t>Back button sudah diperbaiki</t>
+  </si>
+  <si>
+    <t>Checkout button sudah bagus diterapkan</t>
+  </si>
+  <si>
+    <t>Meeting dilaksankan dengan lancar dan baik</t>
+  </si>
+  <si>
+    <t>Sudah selesai</t>
+  </si>
+  <si>
+    <t>Dimulai 10/07/2023</t>
+  </si>
+  <si>
+    <t>Selesai 11/07/2023</t>
+  </si>
+  <si>
+    <t>Saya ingin membuat fitur checkout</t>
+  </si>
+  <si>
+    <t>Saya ingin membuat page notification</t>
+  </si>
+  <si>
+    <t>Supaya user dapat mengetahui status pesanan yang telah dibuat</t>
+  </si>
+  <si>
+    <t>Supaya user dapat mengorder barang yang sudah dimasukkan ke dalam cart</t>
+  </si>
+  <si>
+    <t>Membuat page notifikasi dan fitur checkout</t>
+  </si>
+  <si>
+    <t>Selesai</t>
   </si>
 </sst>
 </file>
@@ -1196,6 +1229,51 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,59 +1307,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1389,14 +1422,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>367392</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>533893</xdr:colOff>
-      <xdr:row>177</xdr:row>
-      <xdr:rowOff>15555</xdr:rowOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>15556</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1439,14 +1472,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>354107</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>323</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>520608</xdr:colOff>
-      <xdr:row>201</xdr:row>
-      <xdr:rowOff>179163</xdr:rowOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>179161</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1489,13 +1522,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>354429</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>27858</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>520930</xdr:colOff>
-      <xdr:row>226</xdr:row>
+      <xdr:row>244</xdr:row>
       <xdr:rowOff>16201</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1845,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B8536-4987-4D23-A1DF-107BD88A4060}">
-  <dimension ref="B1:I164"/>
+  <dimension ref="B1:I182"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1909,16 +1942,16 @@
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="39" t="s">
@@ -1947,10 +1980,10 @@
       </c>
     </row>
     <row r="9" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="54">
+      <c r="B9" s="69">
         <v>5</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="70" t="s">
         <v>87</v>
       </c>
       <c r="D9" s="32" t="s">
@@ -1973,8 +2006,8 @@
       </c>
     </row>
     <row r="10" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="55"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="38" t="s">
         <v>110</v>
       </c>
@@ -1995,18 +2028,18 @@
       </c>
     </row>
     <row r="11" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="69">
+      <c r="B11" s="44">
         <v>13</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="38" t="s">
         <v>110</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G11" s="41" t="s">
         <v>31</v>
@@ -2015,14 +2048,14 @@
         <v>5</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="56">
+      <c r="B12" s="49">
         <v>6</v>
       </c>
-      <c r="C12" s="58"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="36" t="s">
         <v>6</v>
       </c>
@@ -2043,8 +2076,8 @@
       </c>
     </row>
     <row r="13" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="55"/>
-      <c r="C13" s="59"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="38" t="s">
         <v>110</v>
       </c>
@@ -2065,10 +2098,10 @@
       </c>
     </row>
     <row r="14" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="56">
+      <c r="B14" s="49">
         <v>8</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="51" t="s">
         <v>88</v>
       </c>
       <c r="D14" s="36" t="s">
@@ -2091,8 +2124,8 @@
       </c>
     </row>
     <row r="15" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="55"/>
-      <c r="C15" s="58"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="38" t="s">
         <v>110</v>
       </c>
@@ -2113,10 +2146,10 @@
       </c>
     </row>
     <row r="16" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="56">
+      <c r="B16" s="49">
         <v>4</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="36" t="s">
         <v>6</v>
       </c>
@@ -2137,8 +2170,8 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="55"/>
-      <c r="C17" s="59"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="38" t="s">
         <v>110</v>
       </c>
@@ -2159,10 +2192,10 @@
       </c>
     </row>
     <row r="18" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="56">
+      <c r="B18" s="49">
         <v>11</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="51" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="36" t="s">
@@ -2185,8 +2218,8 @@
       </c>
     </row>
     <row r="19" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="55"/>
-      <c r="C19" s="58"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="38" t="s">
         <v>110</v>
       </c>
@@ -2207,10 +2240,10 @@
       </c>
     </row>
     <row r="20" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="56">
+      <c r="B20" s="49">
         <v>2</v>
       </c>
-      <c r="C20" s="58"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="36" t="s">
         <v>6</v>
       </c>
@@ -2231,8 +2264,8 @@
       </c>
     </row>
     <row r="21" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="55"/>
-      <c r="C21" s="58"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="38" t="s">
         <v>110</v>
       </c>
@@ -2253,10 +2286,10 @@
       </c>
     </row>
     <row r="22" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="56">
+      <c r="B22" s="49">
         <v>3</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="36" t="s">
         <v>6</v>
       </c>
@@ -2277,8 +2310,8 @@
       </c>
     </row>
     <row r="23" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="55"/>
-      <c r="C23" s="58"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="38" t="s">
         <v>110</v>
       </c>
@@ -2299,10 +2332,10 @@
       </c>
     </row>
     <row r="24" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="56">
+      <c r="B24" s="49">
         <v>10</v>
       </c>
-      <c r="C24" s="58"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="36" t="s">
         <v>6</v>
       </c>
@@ -2323,8 +2356,8 @@
       </c>
     </row>
     <row r="25" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="55"/>
-      <c r="C25" s="59"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="38" t="s">
         <v>110</v>
       </c>
@@ -2345,10 +2378,10 @@
       </c>
     </row>
     <row r="26" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="56">
+      <c r="B26" s="49">
         <v>1</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="51" t="s">
         <v>90</v>
       </c>
       <c r="D26" s="36" t="s">
@@ -2371,8 +2404,8 @@
       </c>
     </row>
     <row r="27" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="55"/>
-      <c r="C27" s="59"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="38" t="s">
         <v>110</v>
       </c>
@@ -2393,10 +2426,10 @@
       </c>
     </row>
     <row r="28" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="56">
+      <c r="B28" s="49">
         <v>9</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="46" t="s">
         <v>91</v>
       </c>
       <c r="D28" s="36" t="s">
@@ -2419,8 +2452,8 @@
       </c>
     </row>
     <row r="29" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="55"/>
-      <c r="C29" s="71"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="38" t="s">
         <v>110</v>
       </c>
@@ -2441,18 +2474,18 @@
       </c>
     </row>
     <row r="30" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="69">
+      <c r="B30" s="44">
         <v>12</v>
       </c>
-      <c r="C30" s="72"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="38" t="s">
         <v>110</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>35</v>
@@ -2461,14 +2494,14 @@
         <v>8</v>
       </c>
       <c r="I30" s="34" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="56">
+      <c r="B31" s="49">
         <v>7</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="51" t="s">
         <v>92</v>
       </c>
       <c r="D31" s="36" t="s">
@@ -2491,8 +2524,8 @@
       </c>
     </row>
     <row r="32" spans="2:9" s="1" customFormat="1" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="55"/>
-      <c r="C32" s="59"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="38" t="s">
         <v>110</v>
       </c>
@@ -2704,7 +2737,7 @@
         <v>105</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="17"/>
@@ -2817,10 +2850,10 @@
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G65" s="16"/>
       <c r="H65" s="17"/>
@@ -2843,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H67" s="18"/>
     </row>
@@ -2852,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H68" s="18"/>
     </row>
@@ -2861,7 +2894,7 @@
         <v>3</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H69" s="18"/>
     </row>
@@ -2877,7 +2910,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H71" s="18"/>
     </row>
@@ -2886,7 +2919,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H72" s="18"/>
     </row>
@@ -2895,7 +2928,7 @@
         <v>3</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="20"/>
@@ -2911,10 +2944,10 @@
       </c>
       <c r="D75" s="16"/>
       <c r="E75" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G75" s="16"/>
       <c r="H75" s="17"/>
@@ -2937,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H77" s="18"/>
     </row>
@@ -2946,7 +2979,7 @@
         <v>2</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H78" s="18"/>
     </row>
@@ -2955,7 +2988,7 @@
         <v>3</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H79" s="18"/>
     </row>
@@ -2964,7 +2997,7 @@
         <v>4</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H80" s="18"/>
     </row>
@@ -2980,7 +3013,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H82" s="18"/>
     </row>
@@ -2989,7 +3022,7 @@
         <v>2</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H83" s="18"/>
     </row>
@@ -2998,7 +3031,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H84" s="18"/>
     </row>
@@ -3007,7 +3040,7 @@
         <v>4</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D85" s="20"/>
       <c r="E85" s="20"/>
@@ -3015,890 +3048,1058 @@
       <c r="G85" s="20"/>
       <c r="H85" s="21"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="68"/>
-      <c r="C86" s="73"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="74"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C87" s="64" t="s">
+    <row r="86" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="5"/>
+      <c r="C86" s="19"/>
+    </row>
+    <row r="87" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="14"/>
+      <c r="C87" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F87" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87" s="16"/>
+      <c r="H87" s="17"/>
+    </row>
+    <row r="88" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="25"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89" s="28">
+        <v>1</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="28">
+        <v>2</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="H90" s="18"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91" s="28"/>
+      <c r="C91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92" s="30">
+        <v>1</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="H92" s="18"/>
+    </row>
+    <row r="93" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="31">
+        <v>2</v>
+      </c>
+      <c r="C93" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="21"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B94" s="72"/>
+      <c r="C94" s="73"/>
+      <c r="D94" s="74"/>
+      <c r="E94" s="74"/>
+      <c r="F94" s="74"/>
+      <c r="G94" s="74"/>
+      <c r="H94" s="74"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C95" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D87" s="65"/>
-      <c r="E87" s="65"/>
-      <c r="F87" s="65"/>
-      <c r="G87" s="65"/>
-      <c r="H87" s="66"/>
-    </row>
-    <row r="88" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C88" s="4" t="s">
+      <c r="D95" s="54"/>
+      <c r="E95" s="54"/>
+      <c r="F95" s="54"/>
+      <c r="G95" s="54"/>
+      <c r="H95" s="55"/>
+    </row>
+    <row r="96" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C96" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D96" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E96" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F88" s="8" t="s">
+      <c r="F96" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G88" s="8" t="s">
+      <c r="G96" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H88" s="8" t="s">
+      <c r="H96" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C89" s="4">
+    <row r="97" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="4">
         <v>1</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D97" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E97" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F89" s="43">
+      <c r="F97" s="43">
         <v>45043</v>
-      </c>
-      <c r="G89" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H89" s="43">
-        <v>45043</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C90" s="4">
-        <v>2</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F90" s="43">
-        <v>45043</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H90" s="43">
-        <v>45043</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C91" s="4">
-        <v>3</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F91" s="43">
-        <v>45043</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H91" s="43">
-        <v>45043</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C92" s="4">
-        <v>4</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F92" s="43">
-        <v>45044</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H92" s="43">
-        <v>45044</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C93" s="4">
-        <v>5</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F93" s="43">
-        <v>45044</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H93" s="43">
-        <v>45044</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C94" s="4">
-        <v>6</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F94" s="43">
-        <v>45045</v>
-      </c>
-      <c r="G94" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H94" s="43">
-        <v>45045</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C95" s="4">
-        <v>7</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F95" s="43">
-        <v>45045</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H95" s="43">
-        <v>45045</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C96" s="4">
-        <v>8</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F96" s="43">
-        <v>45046</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H96" s="43">
-        <v>45046</v>
-      </c>
-    </row>
-    <row r="97" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C97" s="4">
-        <v>9</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F97" s="43">
-        <v>45046</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H97" s="43">
-        <v>45046</v>
-      </c>
-    </row>
-    <row r="98" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="98" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C98" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F98" s="43">
-        <v>45047</v>
+        <v>45043</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H98" s="43">
-        <v>45047</v>
-      </c>
-    </row>
-    <row r="99" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="C99" s="4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F99" s="43">
-        <v>45048</v>
+        <v>45043</v>
       </c>
       <c r="G99" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H99" s="43">
-        <v>45048</v>
-      </c>
-    </row>
-    <row r="100" spans="3:8" x14ac:dyDescent="0.3">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="C100" s="4">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F100" s="43">
-        <v>45049</v>
+        <v>45044</v>
       </c>
       <c r="G100" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H100" s="43">
-        <v>45049</v>
-      </c>
-    </row>
-    <row r="101" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="C101" s="4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="F101" s="43">
-        <v>45094</v>
+        <v>45044</v>
       </c>
       <c r="G101" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H101" s="43">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="4">
+        <v>6</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F102" s="43">
+        <v>45045</v>
+      </c>
+      <c r="G102" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H102" s="43">
+        <v>45045</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="4">
+        <v>7</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F103" s="43">
+        <v>45045</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H103" s="43">
+        <v>45045</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="4">
+        <v>8</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F104" s="43">
+        <v>45046</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H104" s="43">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="105" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="4">
+        <v>9</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F105" s="43">
+        <v>45046</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H105" s="43">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="4">
+        <v>10</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F106" s="43">
+        <v>45047</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H106" s="43">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="4">
+        <v>11</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F107" s="43">
+        <v>45048</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H107" s="43">
+        <v>45048</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="4">
+        <v>12</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E108" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F108" s="43">
+        <v>45049</v>
+      </c>
+      <c r="G108" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H108" s="43">
+        <v>45049</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="4">
+        <v>13</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F109" s="43">
+        <v>45094</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H109" s="43">
         <v>45108</v>
       </c>
     </row>
-    <row r="102" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C102" s="4">
+    <row r="110" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C110" s="4">
         <v>14</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="D110" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E110" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F110" s="43">
+        <v>45108</v>
+      </c>
+      <c r="G110" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H110" s="43">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C111" s="4">
+        <v>15</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F111" s="43">
+        <v>45117</v>
+      </c>
+      <c r="G111" s="8"/>
+      <c r="H111" s="43">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C113" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="D113" s="71"/>
+      <c r="E113" s="71"/>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C114" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C115" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="D115" s="57"/>
+      <c r="E115" s="57"/>
+    </row>
+    <row r="116" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C116" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C117" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" s="57"/>
+      <c r="E117" s="57"/>
+    </row>
+    <row r="118" spans="3:6" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="C118" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F118" s="5"/>
+    </row>
+    <row r="119" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C119" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E119" s="7"/>
+    </row>
+    <row r="120" spans="3:6" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="C120" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C121" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121" s="57"/>
+      <c r="E121" s="57"/>
+    </row>
+    <row r="122" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C122" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C123" s="10"/>
+      <c r="D123" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="10"/>
+    </row>
+    <row r="124" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C124" s="10"/>
+      <c r="D124" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E124" s="10"/>
+    </row>
+    <row r="125" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C125" s="10"/>
+      <c r="D125" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E125" s="10"/>
+    </row>
+    <row r="126" spans="3:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="C126" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="D126" s="61"/>
+      <c r="E126" s="62"/>
+    </row>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C127" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D127" s="64"/>
+      <c r="E127" s="65"/>
+    </row>
+    <row r="128" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C128" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="129" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C129" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E129" s="10"/>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C130" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E130" s="10"/>
+    </row>
+    <row r="131" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C131" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D131" s="8"/>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C132" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D132" s="8"/>
+      <c r="E132" s="10"/>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C133" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D133" s="8"/>
+      <c r="E133" s="10"/>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C134" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D134" s="64"/>
+      <c r="E134" s="65"/>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C135" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C136" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E136" s="10"/>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C137" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E137" s="10"/>
+    </row>
+    <row r="138" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C138" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D138" s="8"/>
+      <c r="E138" s="10"/>
+    </row>
+    <row r="139" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C139" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="D139" s="64"/>
+      <c r="E139" s="65"/>
+    </row>
+    <row r="140" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C140" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="F102" s="43">
-        <v>45108</v>
-      </c>
-      <c r="G102" s="8" t="s">
+      <c r="D140" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E140" s="4"/>
+    </row>
+    <row r="141" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C141" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="H102" s="43">
-        <v>45117</v>
-      </c>
-    </row>
-    <row r="104" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C104" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="D104" s="61"/>
-      <c r="E104" s="61"/>
-    </row>
-    <row r="105" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C105" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D105" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="106" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C106" s="60" t="s">
+      <c r="D141" s="8"/>
+      <c r="E141" s="10"/>
+    </row>
+    <row r="142" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C142" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D142" s="8"/>
+      <c r="E142" s="10"/>
+    </row>
+    <row r="143" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="10"/>
+    </row>
+    <row r="144" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+    </row>
+    <row r="146" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C146" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D146" s="59"/>
+      <c r="E146" s="59"/>
+      <c r="F146" s="59"/>
+      <c r="G146" s="59"/>
+    </row>
+    <row r="147" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C147" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D147" s="58"/>
+      <c r="E147" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F147" s="58"/>
+      <c r="G147" s="58"/>
+    </row>
+    <row r="148" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C148" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E148" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F148" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G148" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="149" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C149" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D106" s="60"/>
-      <c r="E106" s="60"/>
-    </row>
-    <row r="107" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C107" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="108" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C108" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D108" s="60"/>
-      <c r="E108" s="60"/>
-    </row>
-    <row r="109" spans="3:8" ht="36.6" x14ac:dyDescent="0.3">
-      <c r="C109" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F109" s="5"/>
-    </row>
-    <row r="110" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C110" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E110" s="7"/>
-    </row>
-    <row r="111" spans="3:8" ht="36.6" x14ac:dyDescent="0.3">
-      <c r="C111" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E111" s="7"/>
-    </row>
-    <row r="112" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C112" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="D112" s="60"/>
-      <c r="E112" s="60"/>
-    </row>
-    <row r="113" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C113" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E113" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="114" spans="3:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="C114" s="10"/>
-      <c r="D114" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="10"/>
-    </row>
-    <row r="115" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C115" s="10"/>
-      <c r="D115" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E115" s="10"/>
-    </row>
-    <row r="116" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C116" s="10"/>
-      <c r="D116" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E116" s="10"/>
-    </row>
-    <row r="117" spans="3:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="C117" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="D117" s="46"/>
-      <c r="E117" s="47"/>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C118" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="D118" s="49"/>
-      <c r="E118" s="50"/>
-    </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C119" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="120" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C120" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E120" s="10"/>
-    </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C121" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E121" s="10"/>
-    </row>
-    <row r="122" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C122" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D122" s="8"/>
-      <c r="E122" s="10"/>
-    </row>
-    <row r="123" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C123" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="10"/>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C124" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D124" s="8"/>
-      <c r="E124" s="10"/>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C125" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D125" s="49"/>
-      <c r="E125" s="50"/>
-    </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C126" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E126" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C127" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E127" s="10"/>
-    </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C128" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E128" s="10"/>
-    </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C129" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D129" s="8"/>
-      <c r="E129" s="10"/>
-    </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-    </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C132" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="D132" s="44"/>
-      <c r="E132" s="44"/>
-      <c r="F132" s="44"/>
-      <c r="G132" s="44"/>
-    </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C133" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="D133" s="67"/>
-      <c r="E133" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F133" s="67"/>
-      <c r="G133" s="67"/>
-    </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C134" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E134" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F134" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G134" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C135" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="D135" s="63"/>
-      <c r="E135" s="63"/>
-      <c r="F135" s="63"/>
-      <c r="G135" s="63"/>
-    </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C136" s="4" t="s">
+      <c r="D149" s="45"/>
+      <c r="E149" s="45"/>
+      <c r="F149" s="45"/>
+      <c r="G149" s="45"/>
+    </row>
+    <row r="150" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C150" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D136" s="2" t="s">
+      <c r="D150" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E136" s="2" t="s">
+      <c r="E150" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F136" s="2" t="s">
+      <c r="F150" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G136" s="2" t="s">
+      <c r="G150" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="137" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
-      <c r="G137" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C138" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="D138" s="63"/>
-      <c r="E138" s="63"/>
-      <c r="F138" s="63"/>
-      <c r="G138" s="63"/>
-    </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C139" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="140" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C140" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G140" s="2"/>
-    </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C141" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="D141" s="63"/>
-      <c r="E141" s="63"/>
-      <c r="F141" s="63"/>
-      <c r="G141" s="63"/>
-    </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C142" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G142" s="2"/>
-    </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-    </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
-      <c r="G144" s="2"/>
-    </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C145" s="63" t="s">
-        <v>131</v>
-      </c>
-      <c r="D145" s="63"/>
-      <c r="E145" s="63"/>
-      <c r="F145" s="63"/>
-      <c r="G145" s="63"/>
-    </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C146" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F146" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G146" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
-      <c r="G147" s="2"/>
-    </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
-    </row>
-    <row r="149" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C149" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="D149" s="63"/>
-      <c r="E149" s="63"/>
-      <c r="F149" s="63"/>
-      <c r="G149" s="63"/>
-    </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C150" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G150" s="2"/>
-    </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
-      <c r="G151" s="2"/>
+      <c r="G151" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
-      <c r="G152" s="2"/>
+      <c r="C152" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D152" s="45"/>
+      <c r="E152" s="45"/>
+      <c r="F152" s="45"/>
+      <c r="G152" s="45"/>
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C153" s="5"/>
-      <c r="D153" s="5"/>
-      <c r="E153" s="5"/>
-      <c r="F153" s="5"/>
-      <c r="G153" s="5"/>
-    </row>
-    <row r="154" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C154" s="5" t="s">
+      <c r="C153" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="154" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C154" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G154" s="2"/>
+    </row>
+    <row r="155" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C155" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D155" s="45"/>
+      <c r="E155" s="45"/>
+      <c r="F155" s="45"/>
+      <c r="G155" s="45"/>
+    </row>
+    <row r="156" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C156" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G156" s="2"/>
+    </row>
+    <row r="157" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+    </row>
+    <row r="158" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+    </row>
+    <row r="159" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C159" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="D159" s="45"/>
+      <c r="E159" s="45"/>
+      <c r="F159" s="45"/>
+      <c r="G159" s="45"/>
+    </row>
+    <row r="160" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C160" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G160" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="161" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+    </row>
+    <row r="162" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+    </row>
+    <row r="163" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C163" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D163" s="45"/>
+      <c r="E163" s="45"/>
+      <c r="F163" s="45"/>
+      <c r="G163" s="45"/>
+    </row>
+    <row r="164" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C164" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G164" s="2"/>
+    </row>
+    <row r="165" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+    </row>
+    <row r="166" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+    </row>
+    <row r="167" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C167" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D167" s="45"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="45"/>
+      <c r="G167" s="45"/>
+    </row>
+    <row r="168" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C168" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+    </row>
+    <row r="169" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+    </row>
+    <row r="170" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+    </row>
+    <row r="171" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+      <c r="G171" s="5"/>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C172" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
-      <c r="F154" s="5"/>
-      <c r="G154" s="5"/>
-    </row>
-    <row r="155" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C155" s="5"/>
-      <c r="D155" s="5"/>
-      <c r="E155" s="5"/>
-      <c r="F155" s="5"/>
-      <c r="G155" s="5"/>
-    </row>
-    <row r="156" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C156" s="5"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
-      <c r="F156" s="5"/>
-      <c r="G156" s="5"/>
-    </row>
-    <row r="157" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C157" s="5"/>
-      <c r="D157" s="5"/>
-      <c r="E157" s="5"/>
-      <c r="F157" s="5"/>
-      <c r="G157" s="5"/>
-    </row>
-    <row r="158" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C158" s="5"/>
-      <c r="D158" s="5"/>
-      <c r="E158" s="5"/>
-      <c r="F158" s="5"/>
-      <c r="G158" s="5"/>
-    </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C159" s="5"/>
-      <c r="D159" s="5"/>
-      <c r="E159" s="5"/>
-      <c r="F159" s="5"/>
-      <c r="G159" s="5"/>
-    </row>
-    <row r="160" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C160" s="5"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
-    </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C161" s="5"/>
-      <c r="D161" s="5"/>
-      <c r="E161" s="5"/>
-      <c r="F161" s="5"/>
-      <c r="G161" s="5"/>
-    </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C162" s="5"/>
-      <c r="D162" s="5"/>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
-    </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C163" s="5"/>
-      <c r="D163" s="5"/>
-      <c r="E163" s="5"/>
-      <c r="F163" s="5"/>
-      <c r="G163" s="5"/>
-    </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C164" s="5"/>
-      <c r="D164" s="5"/>
-      <c r="E164" s="5"/>
-      <c r="F164" s="5"/>
-      <c r="G164" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="5"/>
+    </row>
+    <row r="173" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="5"/>
+      <c r="G173" s="5"/>
+    </row>
+    <row r="174" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+      <c r="G174" s="5"/>
+    </row>
+    <row r="175" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="5"/>
+      <c r="G175" s="5"/>
+    </row>
+    <row r="176" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="5"/>
+      <c r="G176" s="5"/>
+    </row>
+    <row r="177" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+      <c r="G177" s="5"/>
+    </row>
+    <row r="178" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="5"/>
+    </row>
+    <row r="179" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="5"/>
+    </row>
+    <row r="180" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="5"/>
+    </row>
+    <row r="181" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="5"/>
+    </row>
+    <row r="182" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+      <c r="G182" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="E133:G133"/>
-    <mergeCell ref="C149:G149"/>
+  <mergeCells count="36">
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C146:G146"/>
+    <mergeCell ref="C126:E126"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="E147:G147"/>
+    <mergeCell ref="C167:G167"/>
+    <mergeCell ref="C163:G163"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C145:G145"/>
+    <mergeCell ref="C159:G159"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C87:H87"/>
+    <mergeCell ref="C95:H95"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C18:C25"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C138:G138"/>
-    <mergeCell ref="C141:G141"/>
-    <mergeCell ref="C135:G135"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C132:G132"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C152:G152"/>
+    <mergeCell ref="C155:G155"/>
+    <mergeCell ref="C149:G149"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:G32">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="medium">

</xml_diff>